<commit_message>
Added more error handling
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santosh\Desktop\Aparna\Selenium\fbLogin\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E642DDA-527C-40A0-8F4A-67DF85286E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16225DC7-7892-43E2-9EF4-BD5DB44A2940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>TestCase</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Alpha@2020</t>
-  </si>
-  <si>
-    <t>prasoona@testcase.com</t>
   </si>
 </sst>
 </file>
@@ -970,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1073,68 +1070,53 @@
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" display="prasoona@testcase.com" xr:uid="{74A2F52D-6B91-4B34-8980-DFECCBEAF284}"/>
+    <hyperlink ref="B8" r:id="rId1" display="prasoona@testcase.com" xr:uid="{74A2F52D-6B91-4B34-8980-DFECCBEAF284}"/>
     <hyperlink ref="B6" r:id="rId2" display="prasoona@testcase.com" xr:uid="{2A784610-4F5E-434A-A52C-F6AEE13F830F}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{2F2DC282-D989-4D1A-9FBF-91314D0EF766}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>